<commit_message>
Update docs for change in abundance required metadata, more tweaks to Test_format_good.xlsx to match
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_format_good.xlsx
+++ b/test/fixtures/Test_format_good.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorme/Research/SAFE/Database/safedata_validator_package/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0DFF46-0D7F-FD46-9656-BE77872F1586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1F786F-FFB5-4B4D-8491-C301AD01A7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7960" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7964" uniqueCount="1350">
   <si>
     <t>SAFE Project ID</t>
   </si>
@@ -5948,7 +5948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -70055,7 +70055,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -70155,6 +70157,18 @@
       <c r="A5" t="s">
         <v>283</v>
       </c>
+      <c r="D5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1349</v>
+      </c>
       <c r="H5" t="s">
         <v>287</v>
       </c>

</xml_diff>

<commit_message>
Updated date extents in Test_format_good.xlsx
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_format_good.xlsx
+++ b/test/fixtures/Test_format_good.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorme/Research/SAFE/Database/safedata_validator_package/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1F786F-FFB5-4B4D-8491-C301AD01A7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590C3D1-C2D4-8242-A4B9-FABA2373C724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,24 @@
     <sheet name="DF" sheetId="4" r:id="rId4"/>
     <sheet name="Incidence" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7964" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7970" uniqueCount="1356">
   <si>
     <t>SAFE Project ID</t>
   </si>
@@ -4075,14 +4087,33 @@
   </si>
   <si>
     <t>count of individuals</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>North</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -4113,10 +4144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4419,11 +4451,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4445,7 +4484,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>43346</v>
       </c>
     </row>
@@ -4621,6 +4660,54 @@
       </c>
       <c r="C21" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B22" s="3">
+        <v>41061</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B23" s="3">
+        <v>41120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B24">
+        <v>116.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B25">
+        <v>117.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B26">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B27">
+        <v>5.07</v>
       </c>
     </row>
   </sheetData>
@@ -4630,6 +4717,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5579,6 +5667,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5946,6 +6035,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U1038"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5953,6 +6043,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -70053,13 +70146,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>